<commit_message>
Added Macros to fill blank cells and calculate total targets mastered and in progress
</commit_message>
<xml_diff>
--- a/Standards Progress Tracking - 6th Grade.xlsx
+++ b/Standards Progress Tracking - 6th Grade.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kenne\GitHub\CA_State_Standards_Progress_Tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991A0961-0F1D-4AEF-A570-8ECD42C5A4E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C9426C-B4F7-42D1-9084-C2F724AF5ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20910" yWindow="4600" windowWidth="13090" windowHeight="15450" xr2:uid="{DE98C1BA-3560-4C95-AA9A-227D424B16B3}"/>
+    <workbookView xWindow="21250" yWindow="4940" windowWidth="13090" windowHeight="15450" xr2:uid="{DE98C1BA-3560-4C95-AA9A-227D424B16B3}"/>
   </bookViews>
   <sheets>
     <sheet name="ELA" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="11" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -186,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -209,23 +209,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -369,7 +357,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8F54777B-92D8-46F5-B721-7459CFC8BA7E}" name="PivotTable1" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8F54777B-92D8-46F5-B721-7459CFC8BA7E}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:A23" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -788,7 +776,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -796,7 +784,7 @@
     <col min="1" max="1" width="26.08984375" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.90625" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="192" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6328125" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="8.7265625" style="6"/>
   </cols>
   <sheetData>
@@ -810,7 +798,7 @@
       <c r="C1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="5" t="s">
         <v>22</v>
       </c>
     </row>
@@ -824,6 +812,9 @@
       <c r="C2" s="8" t="s">
         <v>6</v>
       </c>
+      <c r="D2" s="6" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
@@ -835,6 +826,9 @@
       <c r="C3" s="9" t="s">
         <v>7</v>
       </c>
+      <c r="D3" s="6" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
@@ -857,7 +851,7 @@
       <c r="C5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="11" t="b">
+      <c r="D5" s="6" t="b">
         <v>1</v>
       </c>
     </row>
@@ -871,9 +865,6 @@
       <c r="C6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="11" t="b">
-        <v>0</v>
-      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
@@ -918,7 +909,7 @@
       <c r="C10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="11" t="b">
+      <c r="D10" s="6" t="b">
         <v>1</v>
       </c>
     </row>
@@ -987,10 +978,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>